<commit_message>
Starting to look for a correlation with clay and MAP.
</commit_message>
<xml_diff>
--- a/Ecosystem carbon/02BulkSoil.xlsx
+++ b/Ecosystem carbon/02BulkSoil.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vildehaukenes/Documents/GitHub/AfricanBioServices-Vegetation-and-soils/Ecosystem carbon/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vildehaukenes/Google Drive/Skole/Masteroppgave /01Data /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDDBF186-D66F-024B-B301-E3347DFA2B84}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF808107-A9F3-F44B-95CE-9930C5D2107B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16480" xr2:uid="{ADEBF6D1-C104-E94C-AE8D-EDC075A056F2}"/>
   </bookViews>
@@ -30,7 +30,7 @@
     <author>vildehaukenes92@gmail.com</author>
   </authors>
   <commentList>
-    <comment ref="J2" authorId="0" shapeId="0" xr:uid="{3BCA1973-DFF8-EB4D-AC2B-CBE96B518A8C}">
+    <comment ref="K2" authorId="0" shapeId="0" xr:uid="{3BCA1973-DFF8-EB4D-AC2B-CBE96B518A8C}">
       <text>
         <r>
           <rPr>
@@ -64,7 +64,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J10" authorId="0" shapeId="0" xr:uid="{47A1B395-383A-4840-8F49-740848A06759}">
+    <comment ref="K10" authorId="0" shapeId="0" xr:uid="{47A1B395-383A-4840-8F49-740848A06759}">
       <text>
         <r>
           <rPr>
@@ -98,7 +98,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J14" authorId="0" shapeId="0" xr:uid="{AFAE1793-1209-4349-AE69-12899DE92645}">
+    <comment ref="K14" authorId="0" shapeId="0" xr:uid="{AFAE1793-1209-4349-AE69-12899DE92645}">
       <text>
         <r>
           <rPr>
@@ -137,7 +137,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="31">
   <si>
     <t>Region</t>
   </si>
@@ -211,9 +211,6 @@
     <t>Tot_weight_fine_earth_air_dry.g</t>
   </si>
   <si>
-    <t>BD_fine_earth_air_dry</t>
-  </si>
-  <si>
     <t>Average_SubBefore_Dry</t>
   </si>
   <si>
@@ -227,6 +224,12 @@
   </si>
   <si>
     <t>Sand.per</t>
+  </si>
+  <si>
+    <t>BD.controll_g.cm3</t>
+  </si>
+  <si>
+    <t>BD.per.block_A-horizon</t>
   </si>
 </sst>
 </file>
@@ -288,7 +291,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -382,12 +385,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="4" fontId="2" fillId="3" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -417,6 +433,12 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -733,23 +755,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2701036-41A3-AB4C-975A-6EA1841B64A0}">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection sqref="A1:M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.1640625" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" customWidth="1"/>
-    <col min="10" max="10" width="8.1640625" style="11" customWidth="1"/>
-    <col min="11" max="11" width="8.33203125" style="9" customWidth="1"/>
-    <col min="12" max="12" width="8.6640625" style="7" customWidth="1"/>
+    <col min="5" max="6" width="12.83203125" customWidth="1"/>
+    <col min="11" max="11" width="8.1640625" style="11" customWidth="1"/>
+    <col min="12" max="12" width="8.33203125" style="9" customWidth="1"/>
+    <col min="13" max="13" width="8.6640625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -765,29 +787,35 @@
       <c r="E1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -803,34 +831,38 @@
       <c r="E2" s="3">
         <v>100</v>
       </c>
-      <c r="F2" s="5">
-        <f>I2/E2</f>
+      <c r="F2" s="3">
+        <v>1.0724730432719234</v>
+      </c>
+      <c r="G2" s="5">
+        <f t="shared" ref="G2:G16" si="0">J2/E2</f>
         <v>1.0621740084652767</v>
       </c>
-      <c r="G2" s="5">
+      <c r="H2" s="5">
         <v>63.79</v>
       </c>
-      <c r="H2" s="5">
+      <c r="I2" s="5">
         <v>52.08</v>
       </c>
-      <c r="I2" s="3">
-        <f>(H2/G2)*D2</f>
+      <c r="J2" s="3">
+        <f t="shared" ref="J2:J16" si="1">(I2/H2)*D2</f>
         <v>106.21740084652767</v>
       </c>
-      <c r="J2" s="12">
+      <c r="K2" s="12">
         <f>AVERAGE(21,22)</f>
         <v>21.5</v>
       </c>
-      <c r="K2" s="13">
+      <c r="L2" s="13">
         <f>AVERAGE(14,18)</f>
         <v>16</v>
       </c>
-      <c r="L2" s="14">
+      <c r="M2" s="14">
         <f>AVERAGE(65,60)</f>
         <v>62.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O2" s="3"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -846,31 +878,35 @@
       <c r="E3" s="3">
         <v>100</v>
       </c>
-      <c r="F3" s="5">
-        <f t="shared" ref="F3:F16" si="0">I3/E3</f>
+      <c r="F3" s="3">
+        <v>1.0326433095110281</v>
+      </c>
+      <c r="G3" s="5">
+        <f t="shared" si="0"/>
         <v>1.0540579478149512</v>
       </c>
-      <c r="G3" s="5">
+      <c r="H3" s="5">
         <v>62.47</v>
       </c>
-      <c r="H3" s="5">
+      <c r="I3" s="5">
         <v>56.04</v>
       </c>
-      <c r="I3" s="3">
-        <f t="shared" ref="I3:I16" si="1">(H3/G3)*D3</f>
+      <c r="J3" s="3">
+        <f t="shared" si="1"/>
         <v>105.40579478149512</v>
       </c>
-      <c r="J3" s="15">
+      <c r="K3" s="15">
         <v>62</v>
       </c>
-      <c r="K3" s="15">
+      <c r="L3" s="15">
         <v>26</v>
       </c>
-      <c r="L3" s="15">
+      <c r="M3" s="15">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O3" s="3"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -886,25 +922,28 @@
       <c r="E4" s="3">
         <v>100</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="3">
+        <v>0.99716541892720478</v>
+      </c>
+      <c r="G4" s="5">
         <f t="shared" si="0"/>
         <v>1.0923084068741291</v>
       </c>
-      <c r="G4" s="5">
+      <c r="H4" s="5">
         <v>64.59</v>
       </c>
-      <c r="H4" s="5">
+      <c r="I4" s="5">
         <v>59.79</v>
       </c>
-      <c r="I4" s="3">
+      <c r="J4" s="3">
         <f t="shared" si="1"/>
         <v>109.23084068741291</v>
       </c>
-      <c r="J4" s="12"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="14"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K4" s="12"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="14"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -920,31 +959,34 @@
       <c r="E5" s="3">
         <v>100</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="3">
+        <v>1.1697705936511433</v>
+      </c>
+      <c r="G5" s="5">
         <f t="shared" si="0"/>
         <v>1.2045986220157028</v>
       </c>
-      <c r="G5" s="5">
+      <c r="H5" s="5">
         <v>62.41</v>
       </c>
-      <c r="H5" s="5">
+      <c r="I5" s="5">
         <v>57.83</v>
       </c>
-      <c r="I5" s="3">
+      <c r="J5" s="3">
         <f t="shared" si="1"/>
         <v>120.45986220157027</v>
       </c>
-      <c r="J5" s="15">
+      <c r="K5" s="15">
         <v>44</v>
       </c>
-      <c r="K5" s="15">
+      <c r="L5" s="15">
         <v>39</v>
       </c>
-      <c r="L5" s="15">
+      <c r="M5" s="15">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -960,31 +1002,35 @@
       <c r="E6" s="3">
         <v>100</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="3">
+        <v>1.3407467078665298</v>
+      </c>
+      <c r="G6" s="5">
         <f t="shared" si="0"/>
         <v>1.3277343297974926</v>
       </c>
-      <c r="G6" s="5">
+      <c r="H6" s="5">
         <v>62.22</v>
       </c>
-      <c r="H6" s="5">
+      <c r="I6" s="5">
         <v>57.73</v>
       </c>
-      <c r="I6" s="3">
+      <c r="J6" s="3">
         <f t="shared" si="1"/>
         <v>132.77343297974926</v>
       </c>
-      <c r="J6" s="15">
+      <c r="K6" s="15">
         <v>34</v>
       </c>
-      <c r="K6" s="15">
+      <c r="L6" s="15">
         <v>20</v>
       </c>
-      <c r="L6" s="15">
+      <c r="M6" s="15">
         <v>46</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O6" s="3"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1000,31 +1046,35 @@
       <c r="E7" s="3">
         <v>100</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="3">
+        <v>1.3603766872610905</v>
+      </c>
+      <c r="G7" s="5">
         <f t="shared" si="0"/>
         <v>1.4784738577484691</v>
       </c>
-      <c r="G7" s="5">
+      <c r="H7" s="5">
         <v>63.69</v>
       </c>
-      <c r="H7" s="5">
+      <c r="I7" s="5">
         <v>59</v>
       </c>
-      <c r="I7" s="3">
+      <c r="J7" s="3">
         <f t="shared" si="1"/>
         <v>147.84738577484691</v>
       </c>
-      <c r="J7" s="15">
+      <c r="K7" s="15">
         <v>28</v>
       </c>
-      <c r="K7" s="15">
+      <c r="L7" s="15">
         <v>27</v>
       </c>
-      <c r="L7" s="15">
+      <c r="M7" s="15">
         <v>46</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O7" s="3"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1040,25 +1090,28 @@
       <c r="E8" s="3">
         <v>100</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="3">
+        <v>1.1158412339665564</v>
+      </c>
+      <c r="G8" s="5">
         <f t="shared" si="0"/>
         <v>1.1740343039999999</v>
       </c>
-      <c r="G8" s="5">
+      <c r="H8" s="5">
         <v>62.5</v>
       </c>
-      <c r="H8" s="5">
+      <c r="I8" s="5">
         <v>55.69</v>
       </c>
-      <c r="I8" s="3">
+      <c r="J8" s="3">
         <f t="shared" si="1"/>
         <v>117.40343039999999</v>
       </c>
-      <c r="J8" s="12"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="14"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K8" s="12"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="14"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1074,31 +1127,34 @@
       <c r="E9" s="3">
         <v>100</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="3">
+        <v>1.4254436144798881</v>
+      </c>
+      <c r="G9" s="5">
         <f t="shared" si="0"/>
         <v>1.4164899070810637</v>
       </c>
-      <c r="G9" s="5">
+      <c r="H9" s="5">
         <v>62.42</v>
       </c>
-      <c r="H9" s="5">
+      <c r="I9" s="5">
         <v>56.86</v>
       </c>
-      <c r="I9" s="3">
+      <c r="J9" s="3">
         <f t="shared" si="1"/>
         <v>141.64899070810637</v>
       </c>
-      <c r="J9" s="15">
+      <c r="K9" s="15">
         <v>16</v>
       </c>
-      <c r="K9" s="15">
+      <c r="L9" s="15">
         <v>18</v>
       </c>
-      <c r="L9" s="15">
+      <c r="M9" s="15">
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1114,31 +1170,35 @@
       <c r="E10" s="3">
         <v>100</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="3">
+        <v>1.4605706341668288</v>
+      </c>
+      <c r="G10" s="5">
         <f t="shared" si="0"/>
         <v>1.2623717494999231</v>
       </c>
-      <c r="G10" s="5">
+      <c r="H10" s="5">
         <v>64.989999999999995</v>
       </c>
-      <c r="H10" s="5">
+      <c r="I10" s="5">
         <v>59.71</v>
       </c>
-      <c r="I10" s="3">
+      <c r="J10" s="3">
         <f t="shared" si="1"/>
         <v>126.23717494999232</v>
       </c>
-      <c r="J10" s="15">
-        <v>20</v>
-      </c>
       <c r="K10" s="15">
         <v>20</v>
       </c>
       <c r="L10" s="15">
+        <v>20</v>
+      </c>
+      <c r="M10" s="15">
         <v>60</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O10" s="3"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1154,31 +1214,35 @@
       <c r="E11" s="3">
         <v>100</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="3">
+        <v>1.3184716816374462</v>
+      </c>
+      <c r="G11" s="5">
         <f t="shared" si="0"/>
         <v>1.4287336104892869</v>
       </c>
-      <c r="G11" s="5">
+      <c r="H11" s="5">
         <v>62.54</v>
       </c>
-      <c r="H11" s="5">
+      <c r="I11" s="5">
         <v>55</v>
       </c>
-      <c r="I11" s="3">
+      <c r="J11" s="3">
         <f t="shared" si="1"/>
         <v>142.8733610489287</v>
       </c>
-      <c r="J11" s="15">
+      <c r="K11" s="15">
         <v>10</v>
       </c>
-      <c r="K11" s="15">
+      <c r="L11" s="15">
         <v>21</v>
       </c>
-      <c r="L11" s="15">
+      <c r="M11" s="15">
         <v>69</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O11" s="3"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1194,31 +1258,34 @@
       <c r="E12" s="3">
         <v>100</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="3">
+        <v>1.4124936039053091</v>
+      </c>
+      <c r="G12" s="5">
         <f t="shared" si="0"/>
         <v>1.4652374265186152</v>
       </c>
-      <c r="G12" s="5">
+      <c r="H12" s="5">
         <v>61.24</v>
       </c>
-      <c r="H12" s="5">
+      <c r="I12" s="5">
         <v>51.54</v>
       </c>
-      <c r="I12" s="3">
+      <c r="J12" s="3">
         <f t="shared" si="1"/>
         <v>146.52374265186151</v>
       </c>
-      <c r="J12" s="15">
+      <c r="K12" s="15">
         <v>12</v>
       </c>
-      <c r="K12" s="15">
+      <c r="L12" s="15">
         <v>21</v>
       </c>
-      <c r="L12" s="15">
+      <c r="M12" s="15">
         <v>67</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1234,31 +1301,34 @@
       <c r="E13" s="3">
         <v>100</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="3">
+        <v>1.1390989227916886</v>
+      </c>
+      <c r="G13" s="5">
         <f t="shared" si="0"/>
         <v>1.1701574569221629</v>
       </c>
-      <c r="G13" s="5">
+      <c r="H13" s="5">
         <v>67.319999999999993</v>
       </c>
-      <c r="H13" s="5">
+      <c r="I13" s="5">
         <v>57.5</v>
       </c>
-      <c r="I13" s="3">
+      <c r="J13" s="3">
         <f t="shared" si="1"/>
         <v>117.01574569221629</v>
       </c>
-      <c r="J13" s="15">
+      <c r="K13" s="15">
         <v>23</v>
       </c>
-      <c r="K13" s="15">
+      <c r="L13" s="15">
         <v>46</v>
       </c>
-      <c r="L13" s="15">
+      <c r="M13" s="15">
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -1274,31 +1344,35 @@
       <c r="E14" s="3">
         <v>100</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="3">
+        <v>0.98966190256039321</v>
+      </c>
+      <c r="G14" s="5">
         <f t="shared" si="0"/>
         <v>1.1911436860589404</v>
       </c>
-      <c r="G14" s="5">
+      <c r="H14" s="5">
         <v>65.489999999999995</v>
       </c>
-      <c r="H14" s="5">
+      <c r="I14" s="5">
         <v>55.72</v>
       </c>
-      <c r="I14" s="3">
+      <c r="J14" s="3">
         <f t="shared" si="1"/>
         <v>119.11436860589403</v>
       </c>
-      <c r="J14" s="15">
+      <c r="K14" s="15">
         <v>21</v>
       </c>
-      <c r="K14" s="15">
+      <c r="L14" s="15">
         <v>36</v>
       </c>
-      <c r="L14" s="15">
+      <c r="M14" s="15">
         <v>44</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O14" s="3"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -1314,31 +1388,35 @@
       <c r="E15" s="3">
         <v>100</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="3">
+        <v>1.1588266521141533</v>
+      </c>
+      <c r="G15" s="5">
         <f t="shared" si="0"/>
         <v>1.163385551818036</v>
       </c>
-      <c r="G15" s="5">
+      <c r="H15" s="5">
         <v>62.43</v>
       </c>
-      <c r="H15" s="5">
+      <c r="I15" s="5">
         <v>53.96</v>
       </c>
-      <c r="I15" s="3">
+      <c r="J15" s="3">
         <f t="shared" si="1"/>
         <v>116.33855518180361</v>
       </c>
-      <c r="J15" s="15">
+      <c r="K15" s="15">
         <v>35</v>
       </c>
-      <c r="K15" s="15">
+      <c r="L15" s="15">
         <v>40</v>
       </c>
-      <c r="L15" s="15">
+      <c r="M15" s="15">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O15" s="3"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -1354,96 +1432,105 @@
       <c r="E16" s="3">
         <v>100</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="3">
+        <v>1.1995414861403799</v>
+      </c>
+      <c r="G16" s="5">
         <f t="shared" si="0"/>
         <v>1.3055968780173799</v>
       </c>
-      <c r="G16" s="5">
+      <c r="H16" s="5">
         <v>62.14</v>
       </c>
-      <c r="H16" s="5">
+      <c r="I16" s="5">
         <v>53.41</v>
       </c>
-      <c r="I16" s="3">
+      <c r="J16" s="3">
         <f t="shared" si="1"/>
         <v>130.55968780173799</v>
       </c>
-      <c r="J16" s="15">
+      <c r="K16" s="15">
         <v>25</v>
       </c>
-      <c r="K16" s="15">
+      <c r="L16" s="15">
         <v>44</v>
       </c>
-      <c r="L16" s="15">
+      <c r="M16" s="15">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="6:12" x14ac:dyDescent="0.2">
-      <c r="F17" s="4"/>
+    <row r="17" spans="7:15" x14ac:dyDescent="0.2">
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
-      <c r="J17" s="14"/>
+      <c r="I17" s="4"/>
       <c r="K17" s="14"/>
       <c r="L17" s="14"/>
-    </row>
-    <row r="18" spans="6:12" x14ac:dyDescent="0.2">
-      <c r="F18" s="4"/>
+      <c r="M17" s="14"/>
+    </row>
+    <row r="18" spans="7:15" x14ac:dyDescent="0.2">
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
-      <c r="J18" s="7"/>
+      <c r="I18" s="4"/>
       <c r="K18" s="7"/>
-    </row>
-    <row r="19" spans="6:12" x14ac:dyDescent="0.2">
-      <c r="J19" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="O18" s="3"/>
+    </row>
+    <row r="19" spans="7:15" x14ac:dyDescent="0.2">
       <c r="K19" s="7"/>
-    </row>
-    <row r="20" spans="6:12" x14ac:dyDescent="0.2">
-      <c r="J20" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="O19" s="3"/>
+    </row>
+    <row r="20" spans="7:15" x14ac:dyDescent="0.2">
       <c r="K20" s="7"/>
-    </row>
-    <row r="21" spans="6:12" x14ac:dyDescent="0.2">
-      <c r="J21" s="7"/>
+      <c r="L20" s="7"/>
+    </row>
+    <row r="21" spans="7:15" x14ac:dyDescent="0.2">
       <c r="K21" s="7"/>
-    </row>
-    <row r="22" spans="6:12" x14ac:dyDescent="0.2">
-      <c r="J22" s="7"/>
+      <c r="L21" s="7"/>
+    </row>
+    <row r="22" spans="7:15" x14ac:dyDescent="0.2">
       <c r="K22" s="7"/>
-    </row>
-    <row r="23" spans="6:12" x14ac:dyDescent="0.2">
-      <c r="J23" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="O22" s="3"/>
+    </row>
+    <row r="23" spans="7:15" x14ac:dyDescent="0.2">
       <c r="K23" s="7"/>
-    </row>
-    <row r="24" spans="6:12" x14ac:dyDescent="0.2">
-      <c r="J24" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="O23" s="3"/>
+    </row>
+    <row r="24" spans="7:15" x14ac:dyDescent="0.2">
       <c r="K24" s="7"/>
-    </row>
-    <row r="25" spans="6:12" x14ac:dyDescent="0.2">
-      <c r="J25" s="7"/>
+      <c r="L24" s="7"/>
+    </row>
+    <row r="25" spans="7:15" x14ac:dyDescent="0.2">
       <c r="K25" s="7"/>
-    </row>
-    <row r="26" spans="6:12" x14ac:dyDescent="0.2">
-      <c r="J26" s="7"/>
+      <c r="L25" s="7"/>
+    </row>
+    <row r="26" spans="7:15" x14ac:dyDescent="0.2">
       <c r="K26" s="7"/>
-    </row>
-    <row r="27" spans="6:12" x14ac:dyDescent="0.2">
-      <c r="J27" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="O26" s="3"/>
+    </row>
+    <row r="27" spans="7:15" x14ac:dyDescent="0.2">
       <c r="K27" s="7"/>
-    </row>
-    <row r="28" spans="6:12" x14ac:dyDescent="0.2">
-      <c r="J28" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="O27" s="3"/>
+    </row>
+    <row r="28" spans="7:15" x14ac:dyDescent="0.2">
       <c r="K28" s="7"/>
-    </row>
-    <row r="29" spans="6:12" x14ac:dyDescent="0.2">
-      <c r="J29" s="7"/>
+      <c r="L28" s="7"/>
+    </row>
+    <row r="29" spans="7:15" x14ac:dyDescent="0.2">
       <c r="K29" s="7"/>
-    </row>
-    <row r="30" spans="6:12" x14ac:dyDescent="0.2">
-      <c r="J30" s="7"/>
+      <c r="L29" s="7"/>
+    </row>
+    <row r="30" spans="7:15" x14ac:dyDescent="0.2">
       <c r="K30" s="7"/>
-    </row>
-    <row r="31" spans="6:12" x14ac:dyDescent="0.2">
-      <c r="J31" s="8"/>
-      <c r="L31" s="10"/>
+      <c r="L30" s="7"/>
+    </row>
+    <row r="31" spans="7:15" x14ac:dyDescent="0.2">
+      <c r="K31" s="8"/>
+      <c r="M31" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>